<commit_message>
loop through the num of people in the list
Looped through the list of wrong questions and updated the column next to it to include all of the messages based on the questions that person got wrong.
</commit_message>
<xml_diff>
--- a/Physics-Test.xlsx
+++ b/Physics-Test.xlsx
@@ -2,41 +2,25 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fae841a71cd6f67/Documents/GitHub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fae841a71cd6f67/Documents/GitHub/Excel_to_outlook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{2D50DEA8-C4A2-4697-A8C6-FAC362F9F70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86D520CA-5E8A-43E4-9BF5-48CBF564F2B3}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1F487037A46A95D83607B1D0500B98B3C1CCA8EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FF130DE-3F21-43EF-B596-0F6A1002EAD2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C54AB77E-60BA-4D84-8C5C-626274216452}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ID numbers</t>
   </si>
@@ -65,9 +49,17 @@
     <t>an953660@ucf.edu</t>
   </si>
   <si>
+    <t>3, 5</t>
+  </si>
+  <si>
     <t>m1</t>
   </si>
   <si>
+    <t xml:space="preserve">m3  
+m5  
+</t>
+  </si>
+  <si>
     <t>m2</t>
   </si>
   <si>
@@ -84,9 +76,6 @@
   </si>
   <si>
     <t>m7</t>
-  </si>
-  <si>
-    <t>3, 5</t>
   </si>
 </sst>
 </file>
@@ -129,11 +118,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -468,11 +460,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DBCA4EE-E7A8-435B-B275-6E88A50CA4B7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,7 +496,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5652828</v>
       </c>
@@ -515,45 +507,48 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{CEC3696D-1007-4B67-8BE7-D2C1FEB0344E}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tested the coe with multiple people to see if the looping through all the people in the list part works
Thank you Aaron!
</commit_message>
<xml_diff>
--- a/Physics-Test.xlsx
+++ b/Physics-Test.xlsx
@@ -461,7 +461,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -540,9 +540,26 @@
       </c>
     </row>
     <row r="3">
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>aa000146@ucf.edu</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2, 5</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>m2</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">m2  
+m5  
+</t>
         </is>
       </c>
     </row>
@@ -584,6 +601,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>